<commit_message>
allow curve extrapolation, added 1Y curve and contributor
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_MainChecks.xlsx
@@ -16,11 +16,11 @@
     <definedName name="AllTriggers">MainChecks!$I$5:$I$5</definedName>
     <definedName name="Currency">MainChecks!$B$1</definedName>
     <definedName name="EvaluationDate">MainChecks!$C$3</definedName>
-    <definedName name="FirstIndex">MainChecks!$B$10</definedName>
+    <definedName name="FirstIndex">MainChecks!$B$11</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!$I$5</definedName>
-    <definedName name="SecondIMMDate">MainChecks!$C$11</definedName>
+    <definedName name="SecondIMMDate">MainChecks!$C$12</definedName>
     <definedName name="Trigger">MainChecks!$I$2</definedName>
-    <definedName name="Yesterday">MainChecks!$C$8</definedName>
+    <definedName name="Yesterday">MainChecks!$C$9</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -578,7 +578,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -694,6 +694,11 @@
     <xf numFmtId="170" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="171" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -788,9 +793,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:22:59</v>
+        <v>Paused at 10:23:23</v>
         <stp/>
-        <stp>{D86EDE08-53D6-4560-BC12-B8C0579384A2}</stp>
+        <stp>{91679897-4589-4761-BB8F-FC7A072CDD7E}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -920,7 +925,7 @@
       <sheetName val="1M (2)"/>
       <sheetName val="3M (2)"/>
       <sheetName val="6M_2"/>
-      <sheetName val="1Y (2)"/>
+      <sheetName val="1Y_2"/>
       <sheetName val="FwdEONIAOIS"/>
       <sheetName val="SFIX3"/>
       <sheetName val="IB365"/>
@@ -933,7 +938,7 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>57</v>
+            <v>13</v>
           </cell>
         </row>
       </sheetData>
@@ -941,14 +946,14 @@
       <sheetData sheetId="2">
         <row r="7">
           <cell r="D7" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="7">
           <cell r="D7" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
       </sheetData>
@@ -1400,7 +1405,7 @@
   <dimension ref="A1:W59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1430,7 @@
       </c>
       <c r="C1" s="3" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 18 2014 11:20:01</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 29 2014 14:47:17</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1468,7 +1473,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="40">
-        <v>41753.472546296296</v>
+        <v>41764.432118055556</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="5"/>
@@ -1492,17 +1497,17 @@
         <v>USDSTD</v>
       </c>
       <c r="C3" s="49">
-        <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41753</v>
+        <f>_xll.qlCalendarAdjust(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
+        <v>41765</v>
       </c>
       <c r="D3" s="17"/>
-      <c r="E3" s="18">
+      <c r="E3" s="18" t="e">
         <f>_xll.qlYieldTSDiscount(B3,C3,,Trigger)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="F3" s="19" t="str">
-        <f>IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
+        <v>qlYieldTSDiscount - 1st iteration: failed at 4th alive instrument, maturity May 14th, 2014, reference date May 6th, 2014: Missing no-fix1W Actual/360 fixing for May 2nd, 2014</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="47" t="s">
@@ -1510,7 +1515,7 @@
       </c>
       <c r="I3" s="46" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Updated at 11:22:59</v>
+        <v>Paused at 10:23:23</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="5"/>
@@ -1535,7 +1540,7 @@
       </c>
       <c r="C4" s="41">
         <f>EvaluationDate</f>
-        <v>41753</v>
+        <v>41765</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18">
@@ -1551,7 +1556,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="45">
-        <v>123.8125</v>
+        <v>124.71875</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="5"/>
@@ -1576,7 +1581,7 @@
       </c>
       <c r="C5" s="41">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D","Following")</f>
-        <v>41757</v>
+        <v>41767</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="18" t="e">
@@ -1585,7 +1590,7 @@
       </c>
       <c r="F5" s="19" t="str">
         <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <v>qlYieldTSDiscount - 1st iteration: failed at 1st alive instrument, maturity May 14th, 2014, reference date May 6th, 2014: Missing no-fix1W Actual/360 fixing for May 2nd, 2014</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="20" t="s">
@@ -1593,7 +1598,7 @@
       </c>
       <c r="I5" s="21">
         <f>[1]!TriggerCounter</f>
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="5"/>
@@ -1618,16 +1623,16 @@
       </c>
       <c r="C6" s="41">
         <f>C5</f>
-        <v>41757</v>
+        <v>41767</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="E6" s="18">
+      <c r="E6" s="18" t="e">
         <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="F6" s="19" t="str">
-        <f>IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
+        <v>qlYieldTSDiscount - 1st iteration: failed at 1st alive instrument, maturity May 14th, 2014, reference date May 7th, 2014: Missing no-fix1W Actual/360 fixing for May 2nd, 2014</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="20" t="s">
@@ -1635,7 +1640,7 @@
       </c>
       <c r="I6" s="21">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>873</v>
+        <v>1271</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5"/>
@@ -1660,7 +1665,7 @@
       </c>
       <c r="C7" s="41">
         <f>C6</f>
-        <v>41757</v>
+        <v>41767</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="e">
@@ -1669,7 +1674,7 @@
       </c>
       <c r="F7" s="19" t="str">
         <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <v>qlYieldTSDiscount - 10th instrument (maturity: May 9th, 2016) has an invalid quote</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="34" t="s">
@@ -1693,21 +1698,24 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="42">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41751</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
+      <c r="B8" s="16" t="str">
+        <f>UPPER(Currency)&amp;"1Y"</f>
+        <v>USD1Y</v>
+      </c>
+      <c r="C8" s="41">
+        <f>C7</f>
+        <v>41767</v>
+      </c>
+      <c r="D8" s="51"/>
+      <c r="E8" s="18" t="e">
+        <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F8" s="15" t="str">
+      <c r="F8" s="19" t="str">
         <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v>qlIndexFixing - Missing USDLibor3M Actual/360 fixing for April 22nd, 2014</v>
+        <v>qlYieldTSDiscount - 8th instrument (maturity: May 9th, 2016) has an invalid quote</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="20" t="s">
@@ -1734,19 +1742,19 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="43">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>41752</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="29" t="e">
+      <c r="B9" s="24"/>
+      <c r="C9" s="42">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
+        <v>41760</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="e">
         <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="19" t="str">
+      <c r="F9" s="15" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixing - Missing USDLibor3M Actual/360 fixing for April 23rd, 2014</v>
+        <v>qlIndexFixing - Missing USDLibor3M Actual/360 fixing for May 1st, 2014</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="22" t="s">
@@ -1773,18 +1781,15 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="27" t="str">
-        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
-        <v>UsdLibor3M</v>
-      </c>
+      <c r="B10" s="27"/>
       <c r="C10" s="43">
-        <f>EvaluationDate</f>
-        <v>41753</v>
-      </c>
-      <c r="D10" s="28"/>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
+        <v>41761</v>
+      </c>
+      <c r="D10" s="36"/>
       <c r="E10" s="29">
         <f>_xll.qlIndexFixing(FirstIndex,C10)</f>
-        <v>2.2589999992241481E-3</v>
+        <v>2.2285E-3</v>
       </c>
       <c r="F10" s="19" t="str">
         <f>IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
@@ -1815,19 +1820,22 @@
     </row>
     <row r="11" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="44">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41897</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32">
-        <f>_xll.qlIndexFixing(FirstIndex,C11,TRUE)</f>
-        <v>2.424999999226738E-3</v>
-      </c>
-      <c r="F11" s="33" t="str">
-        <f>IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
-        <v/>
+      <c r="B11" s="27" t="str">
+        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
+        <v>UsdLibor3M</v>
+      </c>
+      <c r="C11" s="43">
+        <f>EvaluationDate</f>
+        <v>41765</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F11" s="19" t="str">
+        <f ca="1">IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
+        <v>qlIndexFixing - 1st iteration: failed at 1st alive instrument, maturity May 14th, 2014, reference date May 7th, 2014: Missing no-fix1W Actual/360 fixing for May 2nd, 2014</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="34" t="s">
@@ -1853,16 +1861,25 @@
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="44">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>41897</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F12" s="33" t="str">
+        <f ca="1">IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>
+        <v>qlIndexFixing - 1st iteration: failed at 1st alive instrument, maturity May 14th, 2014, reference date May 7th, 2014: Missing no-fix1W Actual/360 fixing for May 2nd, 2014</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1877,17 +1894,17 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+    <row r="13" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -2904,6 +2921,11 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -2920,6 +2942,7 @@
       <c r="W54" s="5"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>

</xml_diff>

<commit_message>
USD modified for UK Holiday + JPY Contributor improvement
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_MainChecks.xlsx
@@ -9,16 +9,13 @@
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Currency">MainChecks!$U$4</definedName>
-    <definedName name="FirstIndex">MainChecks!$K$11</definedName>
+    <definedName name="FirstIndex">MainChecks!$K$10</definedName>
     <definedName name="FuturesDates">MainChecks!$C$14:$C$17</definedName>
     <definedName name="FuturesTable">MainChecks!$A$4:$H$12</definedName>
     <definedName name="IMMFutures">MainChecks!$D$14:$D$17</definedName>
-    <definedName name="InterestRatesTrigger">MainChecks!$Q$8</definedName>
+    <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>ObjectID</t>
   </si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>MarketData Checks</t>
-  </si>
-  <si>
-    <t># Mkt Updates</t>
   </si>
   <si>
     <t>Reference Date</t>
@@ -189,6 +183,9 @@
   </si>
   <si>
     <t>EDM5</t>
+  </si>
+  <si>
+    <t>Stale</t>
   </si>
 </sst>
 </file>
@@ -568,7 +565,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -581,12 +578,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,9 +606,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -651,15 +639,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -799,27 +778,27 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 13:02:04</v>
+        <v>Not Signed In</v>
         <stp/>
-        <stp>{A21DE0D0-FA4D-463E-B4B7-D8F9A9B0A43C}</stp>
+        <stp>{FF59E8C2-1979-43B8-ACB8-1576916FA0B1}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{EF6DAE44-3AA4-4295-9701-A69E825047F1}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 13:02:03</v>
+        <v>Not Signed In</v>
         <stp/>
-        <stp>{C0253A40-C105-422E-BF3D-3F3AFE601905}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 13:02:03</v>
-        <stp/>
-        <stp>{F3A14D5D-94B4-4011-B494-F9E667F96E55}</stp>
+        <stp>{AB390024-FD3C-45DF-87D0-F736E78DC796}</stp>
         <tr r="P7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 13:02:03</v>
+        <v>Not Signed In</v>
         <stp/>
-        <stp>{CA9F3A1D-6682-420A-BE8C-4C4428296473}</stp>
+        <stp>{59FB2CD0-170D-4CE5-AC12-34034DD9577C}</stp>
         <tr r="Q7" s="2"/>
       </tp>
     </main>
@@ -920,212 +899,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="General Settings"/>
-      <sheetName val="Libor"/>
-      <sheetName val="LiborSwapIsdaFixAm"/>
-      <sheetName val="LiborSwapForBasisCalc"/>
-      <sheetName val="LiborSwapIsdaFixPm"/>
-      <sheetName val="BasisSwap1MxM"/>
-      <sheetName val="BasisSwap3M6M"/>
-      <sheetName val="BasisSwapxM12M"/>
-      <sheetName val="Deposits"/>
-      <sheetName val="FRA"/>
-      <sheetName val="Futures1M"/>
-      <sheetName val="Futures3M"/>
-      <sheetName val="ImmFra6M "/>
-      <sheetName val="FuturesHWConvAdj"/>
-      <sheetName val="OIS"/>
-      <sheetName val="Swaps1M"/>
-      <sheetName val="SwapsIMMDated"/>
-      <sheetName val="Swap3M"/>
-      <sheetName val="Swap6M"/>
-      <sheetName val="ON"/>
-      <sheetName val="1M (2)"/>
-      <sheetName val="3M (2)"/>
-      <sheetName val="FwdEONIAOIS"/>
-      <sheetName val="SFIX3"/>
-      <sheetName val="IB365"/>
-      <sheetName val="IBOR"/>
-      <sheetName val="USD_Market"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="7">
-          <cell r="D7">
-            <v>74</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Fwd Curve</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>1L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USDSND_Quote#0000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD1x4F_Quote</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Q4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Q4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>X4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3W</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>X1S</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="7">
-          <cell r="D7">
-            <v>12</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="18">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="21">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="22">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>2X</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-4Y=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="24">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="25">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="26" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1506,13 +1279,13 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="1"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="21"/>
+      <c r="U2" s="19"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1540,17 +1313,17 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
       <c r="R3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1576,52 +1349,52 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="20" t="s">
+      <c r="L4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="14" t="s">
-        <v>18</v>
+      <c r="U4" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1641,55 +1414,55 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="44" t="s">
+      <c r="B5" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="44" t="s">
-        <v>50</v>
+      <c r="F5" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="31">
-        <v>41890</v>
-      </c>
-      <c r="M5" s="32">
-        <v>147.59</v>
-      </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33" t="str">
+      <c r="L5" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 13:02:03</v>
+        <v>Not Signed In</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="14" t="str">
+      <c r="U5" s="12" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
         <v>1_52 / 1.5.0 / 1.5</v>
       </c>
@@ -1711,57 +1484,57 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="27" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="28">
-        <v>42170</v>
-      </c>
-      <c r="M6" s="34">
-        <v>99.47</v>
-      </c>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="35" t="str">
+      <c r="M6" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 13:02:04</v>
+        <v>Not Signed In</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="22" t="s">
+      <c r="T6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="12">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1723</v>
+        <v>1686</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1781,56 +1554,56 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44" t="s">
+      <c r="E7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="F7" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>52</v>
+      <c r="G7" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="27" t="str">
+      <c r="J7" s="21"/>
+      <c r="K7" s="24" t="str">
         <f>Currency&amp;VLOOKUP(Currency,FuturesTable,5,0)&amp;VLOOKUP(Currency,FuturesTable,6,0)&amp;"10Y"</f>
         <v>USDAM3L10Y</v>
       </c>
-      <c r="L7" s="28">
-        <v>41834</v>
-      </c>
-      <c r="M7" s="40" t="str">
+      <c r="L7" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="34" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>2.596/2.626</v>
-      </c>
-      <c r="N7" s="34">
-        <v>2.5960000000000001</v>
-      </c>
-      <c r="O7" s="34">
-        <v>2.6259999999999999</v>
-      </c>
-      <c r="P7" s="34" t="str">
+        <v>Stale/Stale</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 13:02:03</v>
-      </c>
-      <c r="Q7" s="35" t="str">
+        <v>Not Signed In</v>
+      </c>
+      <c r="Q7" s="32" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 13:02:03</v>
+        <v>Not Signed In</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1851,45 +1624,42 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="38">
-        <f>[1]!TriggerCounter</f>
-        <v>74</v>
-      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
       <c r="R8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1910,42 +1680,48 @@
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
     </row>
-    <row r="9" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="F9" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>51</v>
+      <c r="G9" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="13"/>
+      <c r="K9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="R9" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1968,34 +1744,38 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+        <v>22</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="8"/>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="20" t="s">
+      <c r="K10" s="22" t="str">
+        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
+        <v>UsdLibor3M</v>
+      </c>
+      <c r="L10" s="23">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41873</v>
+      </c>
+      <c r="M10" s="33">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>2.3840000000000003E-3</v>
+      </c>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="35" t="str">
+        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v/>
+      </c>
+      <c r="R10" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -2018,38 +1798,38 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="8"/>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="25" t="str">
-        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
-        <v>UsdLibor3M</v>
-      </c>
-      <c r="L11" s="26">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41831</v>
-      </c>
-      <c r="M11" s="39">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>2.3360000000000004E-3</v>
-      </c>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="41" t="str">
-        <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
+      <c r="K11" s="24" t="str">
+        <f>UPPER(Currency)&amp;"STD"</f>
+        <v>USDSTD</v>
+      </c>
+      <c r="L11" s="25">
+        <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
+        <v>41873</v>
+      </c>
+      <c r="M11" s="26">
+        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="36" t="str">
+        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
         <v/>
       </c>
       <c r="R11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -2071,47 +1851,47 @@
       <c r="AJ11" s="3"/>
     </row>
     <row r="12" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="27" t="str">
-        <f>UPPER(Currency)&amp;"STD"</f>
-        <v>USDSTD</v>
-      </c>
-      <c r="L12" s="28">
+      <c r="K12" s="24" t="str">
+        <f>UPPER(Currency)&amp;"ON"</f>
+        <v>USDON</v>
+      </c>
+      <c r="L12" s="25">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>41834</v>
-      </c>
-      <c r="M12" s="29">
+        <v>41873</v>
+      </c>
+      <c r="M12" s="26">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
         <v>1</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="42" t="str">
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="36" t="str">
         <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v/>
       </c>
       <c r="R12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -2143,27 +1923,27 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="27" t="str">
-        <f>UPPER(Currency)&amp;"ON"</f>
-        <v>USDON</v>
-      </c>
-      <c r="L13" s="28">
+      <c r="K13" s="24" t="str">
+        <f>UPPER(Currency)&amp;"1M"</f>
+        <v>USD1M</v>
+      </c>
+      <c r="L13" s="25">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41834</v>
-      </c>
-      <c r="M13" s="29">
+        <v>41878</v>
+      </c>
+      <c r="M13" s="26">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
         <v>1</v>
       </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="42" t="str">
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="37" t="str">
         <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -2189,7 +1969,7 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="39">
         <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
         <v>41899</v>
       </c>
@@ -2203,27 +1983,27 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="27" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>USD1M</v>
-      </c>
-      <c r="L14" s="28">
+      <c r="K14" s="24" t="str">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>USD3M</v>
+      </c>
+      <c r="L14" s="25">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41836</v>
-      </c>
-      <c r="M14" s="29">
+        <v>41878</v>
+      </c>
+      <c r="M14" s="26">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
         <v>1</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="43" t="str">
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="37" t="str">
         <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v/>
       </c>
       <c r="R14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -2246,10 +2026,10 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="48" t="b">
+      <c r="B15" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="40">
         <v>41990</v>
       </c>
       <c r="D15" s="8" t="str">
@@ -2261,27 +2041,27 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="27" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>USD3M</v>
-      </c>
-      <c r="L15" s="28">
+      <c r="K15" s="24" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>USD6M</v>
+      </c>
+      <c r="L15" s="25">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>41836</v>
-      </c>
-      <c r="M15" s="29">
+        <v>41878</v>
+      </c>
+      <c r="M15" s="26">
         <f>_xll.qlYieldTSDiscount(K15,L15)</f>
         <v>1</v>
       </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="43" t="str">
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="37" t="str">
         <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
         <v/>
       </c>
       <c r="R15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -2304,10 +2084,10 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="48" t="b">
+      <c r="B16" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="40">
         <v>42081</v>
       </c>
       <c r="D16" s="8" t="str">
@@ -2319,27 +2099,27 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="27" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>USD6M</v>
-      </c>
-      <c r="L16" s="28">
+      <c r="K16" s="46" t="str">
+        <f>UPPER(Currency)&amp;"1Y"</f>
+        <v>USD1Y</v>
+      </c>
+      <c r="L16" s="47">
         <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>41836</v>
-      </c>
-      <c r="M16" s="29">
+        <v>41878</v>
+      </c>
+      <c r="M16" s="48">
         <f>_xll.qlYieldTSDiscount(K16,L16)</f>
         <v>1</v>
       </c>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="43" t="str">
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="49" t="str">
         <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
         <v/>
       </c>
       <c r="R16" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -2362,10 +2142,10 @@
     </row>
     <row r="17" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="49" t="b">
+      <c r="B17" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="41">
         <v>42172</v>
       </c>
       <c r="D17" s="11" t="str">
@@ -2376,28 +2156,16 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="52" t="str">
-        <f>UPPER(Currency)&amp;"1Y"</f>
-        <v>USD1Y</v>
-      </c>
-      <c r="L17" s="53">
-        <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>41836</v>
-      </c>
-      <c r="M17" s="54">
-        <f>_xll.qlYieldTSDiscount(K17,L17)</f>
-        <v>1</v>
-      </c>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="55" t="str">
-        <f>IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
-        <v/>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>14</v>
+      <c r="J17" s="9"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -2418,7 +2186,7 @@
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
     </row>
-    <row r="18" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2428,17 +2196,15 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="11" t="s">
-        <v>14</v>
-      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -3350,7 +3116,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
+      <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
       <c r="U42" s="1"/>
@@ -3380,14 +3146,14 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
@@ -5574,8 +5340,18 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:36" s="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="1:36" s="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" spans="1:36" s="50" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="1:36" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">

</xml_diff>